<commit_message>
updated 1988 Alabama Alaska
</commit_message>
<xml_diff>
--- a/Output/1988/Alaska/Alaska.xlsx
+++ b/Output/1988/Alaska/Alaska.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -333,6 +333,14 @@
   </si>
   <si>
     <t>note</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>State</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -722,170 +730,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:W67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <v>201000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>29495</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>31965</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1">
         <v>10809</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>9486</v>
       </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1">
         <v>5974</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>2132</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>9742</v>
       </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2">
-        <v>1</v>
+      <c r="P2" t="s">
+        <v>21</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
         <v>93430</v>
       </c>
-      <c r="S2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2">
+      <c r="T2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2">
         <v>54</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>465</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>31413</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>100</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
       <c r="J3" t="s">
         <v>21</v>
       </c>
@@ -904,45 +919,48 @@
       <c r="O3" t="s">
         <v>21</v>
       </c>
-      <c r="P3">
-        <v>1</v>
+      <c r="P3" t="s">
+        <v>21</v>
       </c>
       <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
       </c>
-      <c r="T3">
+      <c r="T3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3">
         <v>13</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>3200</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>24838</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>644</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I4" t="s">
@@ -966,50 +984,53 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="P4">
-        <v>0</v>
+      <c r="P4" t="s">
+        <v>21</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>659</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>700</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>12</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
         <v>3500</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>28430</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>810</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
       <c r="J5" t="s">
         <v>21</v>
       </c>
@@ -1028,56 +1049,59 @@
       <c r="O5" t="s">
         <v>21</v>
       </c>
-      <c r="P5">
-        <v>1</v>
+      <c r="P5" t="s">
+        <v>21</v>
       </c>
       <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1250</v>
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
       </c>
       <c r="S5" s="1">
         <v>1250</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="1">
+        <v>1250</v>
+      </c>
+      <c r="U5">
         <v>20</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
         <v>2200</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>24929</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>592</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>333</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>42</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>124</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>214</v>
       </c>
-      <c r="K6" t="s">
-        <v>21</v>
-      </c>
       <c r="L6" t="s">
         <v>21</v>
       </c>
@@ -1090,50 +1114,53 @@
       <c r="O6" t="s">
         <v>21</v>
       </c>
-      <c r="P6">
-        <v>1</v>
+      <c r="P6" t="s">
+        <v>21</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
         <v>800</v>
       </c>
-      <c r="S6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T6">
+      <c r="T6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U6">
         <v>35</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
         <v>2010</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>31079</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>320</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
       <c r="J7" t="s">
         <v>21</v>
       </c>
@@ -1152,56 +1179,59 @@
       <c r="O7" t="s">
         <v>21</v>
       </c>
-      <c r="P7">
-        <v>1</v>
+      <c r="P7" t="s">
+        <v>21</v>
       </c>
       <c r="Q7">
         <v>1</v>
       </c>
       <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
         <v>635</v>
       </c>
-      <c r="S7" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7">
+      <c r="T7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U7">
         <v>33</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>60000</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>29113</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>8978</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1">
         <v>1188</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>1497</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>3363</v>
       </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
       <c r="L8" t="s">
         <v>21</v>
       </c>
@@ -1214,50 +1244,53 @@
       <c r="O8" t="s">
         <v>21</v>
       </c>
-      <c r="P8">
-        <v>1</v>
+      <c r="P8" t="s">
+        <v>21</v>
       </c>
       <c r="Q8">
         <v>1</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1">
         <v>10700</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>30000</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>35</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>765</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>30773</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>213</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
       <c r="J9" t="s">
         <v>21</v>
       </c>
@@ -1276,50 +1309,53 @@
       <c r="O9" t="s">
         <v>21</v>
       </c>
-      <c r="P9">
-        <v>1</v>
+      <c r="P9" t="s">
+        <v>21</v>
       </c>
       <c r="Q9">
         <v>1</v>
       </c>
       <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
         <v>195</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>420</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>60</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>30987</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>498</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
       <c r="J10" t="s">
         <v>21</v>
       </c>
@@ -1338,56 +1374,59 @@
       <c r="O10" t="s">
         <v>21</v>
       </c>
-      <c r="P10">
-        <v>1</v>
+      <c r="P10" t="s">
+        <v>21</v>
       </c>
       <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
       </c>
       <c r="S10" t="s">
         <v>21</v>
       </c>
-      <c r="T10">
+      <c r="T10" t="s">
+        <v>21</v>
+      </c>
+      <c r="U10">
         <v>10</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>31868</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>94</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11">
+      <c r="H11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11">
         <v>62</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>37</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>64</v>
       </c>
-      <c r="K11" t="s">
-        <v>21</v>
-      </c>
       <c r="L11" t="s">
         <v>21</v>
       </c>
@@ -1400,50 +1439,53 @@
       <c r="O11" t="s">
         <v>21</v>
       </c>
-      <c r="P11">
-        <v>1</v>
+      <c r="P11" t="s">
+        <v>21</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
         <v>550</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>970</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>36</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <v>1200</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>26512</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>300</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12">
+      <c r="H12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12">
         <v>300</v>
       </c>
-      <c r="I12" t="s">
-        <v>21</v>
-      </c>
       <c r="J12" t="s">
         <v>21</v>
       </c>
@@ -1462,50 +1504,53 @@
       <c r="O12" t="s">
         <v>21</v>
       </c>
-      <c r="P12">
-        <v>1</v>
+      <c r="P12" t="s">
+        <v>21</v>
       </c>
       <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
       </c>
       <c r="S12" t="s">
         <v>21</v>
       </c>
-      <c r="T12">
+      <c r="T12" t="s">
+        <v>21</v>
+      </c>
+      <c r="U12">
         <v>13</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="D13">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>748</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>25447</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>65</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="H13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
         <v>23</v>
       </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
       <c r="J13" t="s">
         <v>21</v>
       </c>
@@ -1524,50 +1569,53 @@
       <c r="O13" t="s">
         <v>21</v>
       </c>
-      <c r="P13">
-        <v>0</v>
+      <c r="P13" t="s">
+        <v>21</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13" t="s">
-        <v>21</v>
+      <c r="R13">
+        <v>0</v>
       </c>
       <c r="S13" t="s">
         <v>21</v>
       </c>
       <c r="T13" t="s">
+        <v>21</v>
+      </c>
+      <c r="U13" t="s">
         <v>45</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>30742</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="H14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
         <v>23</v>
       </c>
-      <c r="I14" t="s">
-        <v>21</v>
-      </c>
       <c r="J14" t="s">
         <v>21</v>
       </c>
@@ -1586,118 +1634,124 @@
       <c r="O14" t="s">
         <v>21</v>
       </c>
-      <c r="P14">
-        <v>1</v>
+      <c r="P14" t="s">
+        <v>21</v>
       </c>
       <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
       </c>
       <c r="S14" t="s">
         <v>21</v>
       </c>
-      <c r="T14">
+      <c r="T14" t="s">
+        <v>21</v>
+      </c>
+      <c r="U14">
         <v>10</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>26000</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>24108</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>6356</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15">
+      <c r="H15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15">
         <v>530</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>880</v>
       </c>
-      <c r="J15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15">
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15">
         <v>200</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>340</v>
       </c>
-      <c r="M15" t="s">
-        <v>21</v>
-      </c>
       <c r="N15" t="s">
         <v>21</v>
       </c>
       <c r="O15" t="s">
         <v>21</v>
       </c>
-      <c r="P15">
-        <v>1</v>
+      <c r="P15" t="s">
+        <v>21</v>
       </c>
       <c r="Q15">
         <v>1</v>
       </c>
-      <c r="R15" s="1">
-        <v>9400</v>
+      <c r="R15">
+        <v>1</v>
       </c>
       <c r="S15" s="1">
         <v>9400</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="1">
+        <v>9400</v>
+      </c>
+      <c r="U15">
         <v>31</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
         <v>25282</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>30651</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>1506</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16">
+      <c r="H16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16">
         <v>553</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>534</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>917</v>
       </c>
-      <c r="K16" t="s">
-        <v>21</v>
-      </c>
       <c r="L16" t="s">
         <v>21</v>
       </c>
@@ -1710,56 +1764,59 @@
       <c r="O16" t="s">
         <v>21</v>
       </c>
-      <c r="P16">
-        <v>1</v>
+      <c r="P16" t="s">
+        <v>21</v>
       </c>
       <c r="Q16">
         <v>1</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" s="1">
         <v>4063</v>
       </c>
-      <c r="S16" t="s">
-        <v>21</v>
-      </c>
-      <c r="T16">
+      <c r="T16" t="s">
+        <v>21</v>
+      </c>
+      <c r="U16">
         <v>36</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <v>13500</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>19674</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>3566</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17">
+      <c r="H17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17">
         <v>890</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>958</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>1344</v>
       </c>
-      <c r="K17" t="s">
-        <v>21</v>
-      </c>
       <c r="L17" t="s">
         <v>21</v>
       </c>
@@ -1772,45 +1829,48 @@
       <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="P17">
-        <v>1</v>
+      <c r="P17" t="s">
+        <v>21</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1">
         <v>5037</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <v>5047</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>30</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="D18">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>460</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>30987</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>123</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="H18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I18" t="s">
@@ -1834,50 +1894,53 @@
       <c r="O18" t="s">
         <v>21</v>
       </c>
-      <c r="P18">
-        <v>1</v>
+      <c r="P18" t="s">
+        <v>21</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
         <v>123</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>125</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>36</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>31017</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="H19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
         <v>23</v>
       </c>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
       <c r="J19" t="s">
         <v>21</v>
       </c>
@@ -1896,56 +1959,59 @@
       <c r="O19" t="s">
         <v>21</v>
       </c>
-      <c r="P19">
-        <v>1</v>
+      <c r="P19" t="s">
+        <v>21</v>
       </c>
       <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
       </c>
       <c r="S19" t="s">
         <v>21</v>
       </c>
-      <c r="T19">
+      <c r="T19" t="s">
+        <v>21</v>
+      </c>
+      <c r="U19">
         <v>10</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" t="s">
         <v>60</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
         <v>8000</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>25385</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>2312</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>1249</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>182</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>477</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>763</v>
       </c>
-      <c r="K20" t="s">
-        <v>21</v>
-      </c>
       <c r="L20" t="s">
         <v>21</v>
       </c>
@@ -1958,56 +2024,59 @@
       <c r="O20" t="s">
         <v>21</v>
       </c>
-      <c r="P20">
-        <v>1</v>
+      <c r="P20" t="s">
+        <v>21</v>
       </c>
       <c r="Q20">
         <v>1</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1">
         <v>3050</v>
       </c>
-      <c r="S20" s="1">
+      <c r="T20" s="1">
         <v>3400</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>35</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
         <v>2000</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>26665</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>482</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>349</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>84</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>113</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>258</v>
       </c>
-      <c r="K21" t="s">
-        <v>21</v>
-      </c>
       <c r="L21" t="s">
         <v>21</v>
       </c>
@@ -2020,50 +2089,53 @@
       <c r="O21" t="s">
         <v>21</v>
       </c>
-      <c r="P21">
-        <v>1</v>
+      <c r="P21" t="s">
+        <v>21</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
         <v>670</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>800</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>35</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="D22">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>583</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>31778</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>94</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22">
+      <c r="H22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22">
         <v>70</v>
       </c>
-      <c r="I22" t="s">
-        <v>21</v>
-      </c>
       <c r="J22" t="s">
         <v>21</v>
       </c>
@@ -2082,53 +2154,56 @@
       <c r="O22" t="s">
         <v>21</v>
       </c>
-      <c r="P22">
-        <v>1</v>
+      <c r="P22" t="s">
+        <v>21</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="S22">
         <v>200</v>
       </c>
       <c r="T22">
+        <v>200</v>
+      </c>
+      <c r="U22">
         <v>12</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
         <v>3000</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>25965</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>762</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>485</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>119</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>276</v>
       </c>
-      <c r="J23" t="s">
-        <v>21</v>
-      </c>
       <c r="K23" t="s">
         <v>21</v>
       </c>
@@ -2144,56 +2219,59 @@
       <c r="O23" t="s">
         <v>21</v>
       </c>
-      <c r="P23">
-        <v>1</v>
+      <c r="P23" t="s">
+        <v>21</v>
       </c>
       <c r="Q23">
         <v>1</v>
       </c>
       <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
         <v>850</v>
       </c>
-      <c r="S23" s="1">
+      <c r="T23" s="1">
         <v>1000</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>35</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>30256</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>390</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24">
+      <c r="H24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24">
         <v>149</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>190</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>231</v>
       </c>
-      <c r="K24" t="s">
-        <v>21</v>
-      </c>
       <c r="L24" t="s">
         <v>21</v>
       </c>
@@ -2206,50 +2284,53 @@
       <c r="O24" t="s">
         <v>21</v>
       </c>
-      <c r="P24">
-        <v>1</v>
+      <c r="P24" t="s">
+        <v>21</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
-      <c r="R24" s="1">
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1">
         <v>1386</v>
       </c>
-      <c r="S24" s="1">
+      <c r="T24" s="1">
         <v>2500</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>35</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>30225</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>2850</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="H25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="1">
         <v>2400</v>
       </c>
-      <c r="I25" t="s">
-        <v>21</v>
-      </c>
       <c r="J25" t="s">
         <v>21</v>
       </c>
@@ -2268,56 +2349,59 @@
       <c r="O25" t="s">
         <v>21</v>
       </c>
-      <c r="P25">
-        <v>1</v>
+      <c r="P25" t="s">
+        <v>21</v>
       </c>
       <c r="Q25">
         <v>1</v>
       </c>
-      <c r="R25" s="1">
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25" s="1">
         <v>7000</v>
       </c>
-      <c r="S25" t="s">
-        <v>21</v>
-      </c>
-      <c r="T25">
+      <c r="T25" t="s">
+        <v>21</v>
+      </c>
+      <c r="U25">
         <v>39</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
         <v>72</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
         <v>2800</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <v>25082</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>704</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="3">
         <v>355</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>34</v>
       </c>
-      <c r="I26">
-        <v>103</v>
-      </c>
       <c r="J26">
+        <v>103</v>
+      </c>
+      <c r="K26">
         <v>127</v>
       </c>
-      <c r="K26" t="s">
-        <v>21</v>
-      </c>
       <c r="L26" t="s">
         <v>21</v>
       </c>
@@ -2330,45 +2414,48 @@
       <c r="O26" t="s">
         <v>21</v>
       </c>
-      <c r="P26">
-        <v>1</v>
+      <c r="P26" t="s">
+        <v>21</v>
       </c>
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1">
         <v>1000</v>
       </c>
-      <c r="S26" t="s">
-        <v>21</v>
-      </c>
-      <c r="T26">
+      <c r="T26" t="s">
+        <v>21</v>
+      </c>
+      <c r="U26">
         <v>35</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
         <v>73</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="D27">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>250</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>100</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>59</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I27" t="s">
@@ -2392,50 +2479,53 @@
       <c r="O27" t="s">
         <v>21</v>
       </c>
-      <c r="P27">
-        <v>0</v>
+      <c r="P27" t="s">
+        <v>21</v>
       </c>
       <c r="Q27">
         <v>0</v>
       </c>
       <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
         <v>60</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>150</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>12</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
         <v>74</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>30987</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="H28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
         <v>23</v>
       </c>
-      <c r="I28" t="s">
-        <v>21</v>
-      </c>
       <c r="J28" t="s">
         <v>21</v>
       </c>
@@ -2454,50 +2544,53 @@
       <c r="O28" t="s">
         <v>21</v>
       </c>
-      <c r="P28">
-        <v>1</v>
+      <c r="P28" t="s">
+        <v>21</v>
       </c>
       <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
       </c>
       <c r="S28" t="s">
         <v>21</v>
       </c>
-      <c r="T28">
+      <c r="T28" t="s">
+        <v>21</v>
+      </c>
+      <c r="U28">
         <v>10</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
         <v>77</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="D29">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29">
         <v>382</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>30926</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="H29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" t="s">
         <v>23</v>
       </c>
-      <c r="I29" t="s">
-        <v>21</v>
-      </c>
       <c r="J29" t="s">
         <v>21</v>
       </c>
@@ -2516,50 +2609,53 @@
       <c r="O29" t="s">
         <v>21</v>
       </c>
-      <c r="P29">
-        <v>1</v>
+      <c r="P29" t="s">
+        <v>21</v>
       </c>
       <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
       </c>
       <c r="S29" t="s">
         <v>21</v>
       </c>
-      <c r="T29">
+      <c r="T29" t="s">
+        <v>21</v>
+      </c>
+      <c r="U29">
         <v>10</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="D30">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>491</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>30773</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="H30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="s">
         <v>23</v>
       </c>
-      <c r="I30" t="s">
-        <v>21</v>
-      </c>
       <c r="J30" t="s">
         <v>21</v>
       </c>
@@ -2578,59 +2674,62 @@
       <c r="O30" t="s">
         <v>21</v>
       </c>
-      <c r="P30">
-        <v>1</v>
+      <c r="P30" t="s">
+        <v>21</v>
       </c>
       <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
       </c>
       <c r="S30" t="s">
         <v>21</v>
       </c>
-      <c r="T30">
+      <c r="T30" t="s">
+        <v>21</v>
+      </c>
+      <c r="U30">
         <v>10</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
         <v>80</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>31933</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>246</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31">
+      <c r="H31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31">
         <v>35</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>52</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>109</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>25</v>
       </c>
-      <c r="L31" t="s">
-        <v>21</v>
-      </c>
       <c r="M31" t="s">
         <v>21</v>
       </c>
@@ -2640,56 +2739,59 @@
       <c r="O31" t="s">
         <v>21</v>
       </c>
-      <c r="P31">
-        <v>1</v>
+      <c r="P31" t="s">
+        <v>21</v>
       </c>
       <c r="Q31">
         <v>1</v>
       </c>
-      <c r="R31" s="1">
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1">
         <v>1100</v>
       </c>
-      <c r="S31" t="s">
-        <v>21</v>
-      </c>
       <c r="T31" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="U31" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
         <v>81</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
         <v>9000</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="2">
         <v>21869</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>2176</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32">
+      <c r="H32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32">
         <v>541</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>596</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>911</v>
       </c>
-      <c r="K32" t="s">
-        <v>21</v>
-      </c>
       <c r="L32" t="s">
         <v>21</v>
       </c>
@@ -2702,50 +2804,53 @@
       <c r="O32" t="s">
         <v>21</v>
       </c>
-      <c r="P32">
-        <v>1</v>
+      <c r="P32" t="s">
+        <v>21</v>
       </c>
       <c r="Q32">
         <v>1</v>
       </c>
-      <c r="R32" s="1">
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1">
         <v>2690</v>
       </c>
-      <c r="S32" s="1">
+      <c r="T32" s="1">
         <v>2700</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>28</v>
       </c>
-      <c r="U32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
         <v>83</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="D33">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33">
         <v>675</v>
       </c>
-      <c r="E33" s="2">
+      <c r="F33" s="2">
         <v>23743</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>83</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33">
+      <c r="H33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33">
         <v>49</v>
       </c>
-      <c r="I33" t="s">
-        <v>21</v>
-      </c>
       <c r="J33" t="s">
         <v>21</v>
       </c>
@@ -2764,50 +2869,53 @@
       <c r="O33" t="s">
         <v>21</v>
       </c>
-      <c r="P33">
-        <v>1</v>
+      <c r="P33" t="s">
+        <v>21</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33">
-        <v>277</v>
+        <v>0</v>
       </c>
       <c r="S33">
         <v>277</v>
       </c>
       <c r="T33">
+        <v>277</v>
+      </c>
+      <c r="U33">
         <v>12</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
         <v>84</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
         <v>2320</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>31472</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>1450</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="H34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" t="s">
         <v>23</v>
       </c>
-      <c r="I34" t="s">
-        <v>21</v>
-      </c>
       <c r="J34" t="s">
         <v>21</v>
       </c>
@@ -2826,50 +2934,53 @@
       <c r="O34" t="s">
         <v>21</v>
       </c>
-      <c r="P34">
-        <v>1</v>
+      <c r="P34" t="s">
+        <v>21</v>
       </c>
       <c r="Q34">
         <v>1</v>
       </c>
-      <c r="R34" t="s">
-        <v>21</v>
+      <c r="R34">
+        <v>1</v>
       </c>
       <c r="S34" t="s">
         <v>21</v>
       </c>
       <c r="T34" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="U34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
         <v>85</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="D35">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="E35">
         <v>388</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>31747</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>40</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="H35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" t="s">
         <v>23</v>
       </c>
-      <c r="I35" t="s">
-        <v>21</v>
-      </c>
       <c r="J35" t="s">
         <v>21</v>
       </c>
@@ -2888,45 +2999,48 @@
       <c r="O35" t="s">
         <v>21</v>
       </c>
-      <c r="P35">
-        <v>1</v>
+      <c r="P35" t="s">
+        <v>21</v>
       </c>
       <c r="Q35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
         <v>100</v>
       </c>
-      <c r="S35" t="s">
-        <v>21</v>
-      </c>
-      <c r="T35">
+      <c r="T35" t="s">
+        <v>21</v>
+      </c>
+      <c r="U35">
         <v>12</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
         <v>86</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="D36">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="E36">
         <v>350</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>28920</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>86</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="H36" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I36" t="s">
@@ -2950,50 +3064,53 @@
       <c r="O36" t="s">
         <v>21</v>
       </c>
-      <c r="P36">
-        <v>1</v>
+      <c r="P36" t="s">
+        <v>21</v>
       </c>
       <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36" t="s">
-        <v>21</v>
-      </c>
-      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36" t="s">
+        <v>21</v>
+      </c>
+      <c r="T36">
         <v>86</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>12</v>
       </c>
-      <c r="U36" t="s">
+      <c r="V36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
         <v>87</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="D37">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>470</v>
       </c>
-      <c r="E37" s="2">
+      <c r="F37" s="2">
         <v>30742</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="H37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" t="s">
         <v>23</v>
       </c>
-      <c r="I37" t="s">
-        <v>21</v>
-      </c>
       <c r="J37" t="s">
         <v>21</v>
       </c>
@@ -3012,50 +3129,53 @@
       <c r="O37" t="s">
         <v>21</v>
       </c>
-      <c r="P37">
-        <v>1</v>
+      <c r="P37" t="s">
+        <v>21</v>
       </c>
       <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
       </c>
       <c r="S37" t="s">
         <v>21</v>
       </c>
-      <c r="T37">
+      <c r="T37" t="s">
+        <v>21</v>
+      </c>
+      <c r="U37">
         <v>10</v>
       </c>
-      <c r="U37" t="s">
+      <c r="V37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
         <v>88</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="2">
+      <c r="F38" s="2">
         <v>30987</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="H38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" t="s">
         <v>23</v>
       </c>
-      <c r="I38" t="s">
-        <v>21</v>
-      </c>
       <c r="J38" t="s">
         <v>21</v>
       </c>
@@ -3074,50 +3194,53 @@
       <c r="O38" t="s">
         <v>21</v>
       </c>
-      <c r="P38">
-        <v>1</v>
+      <c r="P38" t="s">
+        <v>21</v>
       </c>
       <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
       </c>
       <c r="S38" t="s">
         <v>21</v>
       </c>
-      <c r="T38">
+      <c r="T38" t="s">
+        <v>21</v>
+      </c>
+      <c r="U38">
         <v>10</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
         <v>90</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="2">
+      <c r="F39" s="2">
         <v>30956</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>89</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="H39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" t="s">
         <v>23</v>
       </c>
-      <c r="I39" t="s">
-        <v>21</v>
-      </c>
       <c r="J39" t="s">
         <v>21</v>
       </c>
@@ -3136,50 +3259,53 @@
       <c r="O39" t="s">
         <v>21</v>
       </c>
-      <c r="P39">
-        <v>1</v>
+      <c r="P39" t="s">
+        <v>21</v>
       </c>
       <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
       </c>
       <c r="S39" t="s">
         <v>21</v>
       </c>
-      <c r="T39">
+      <c r="T39" t="s">
+        <v>21</v>
+      </c>
+      <c r="U39">
         <v>10</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" t="s">
         <v>91</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="2">
+      <c r="F40" s="2">
         <v>31291</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>89</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="H40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" t="s">
         <v>23</v>
       </c>
-      <c r="I40" t="s">
-        <v>21</v>
-      </c>
       <c r="J40" t="s">
         <v>21</v>
       </c>
@@ -3198,50 +3324,53 @@
       <c r="O40" t="s">
         <v>21</v>
       </c>
-      <c r="P40">
-        <v>1</v>
+      <c r="P40" t="s">
+        <v>21</v>
       </c>
       <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
       </c>
       <c r="S40" t="s">
         <v>21</v>
       </c>
-      <c r="T40">
+      <c r="T40" t="s">
+        <v>21</v>
+      </c>
+      <c r="U40">
         <v>10</v>
       </c>
-      <c r="U40" t="s">
+      <c r="V40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
         <v>92</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
         <v>1922</v>
       </c>
-      <c r="E41" s="2">
+      <c r="F41" s="2">
         <v>31017</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>200</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="H41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" t="s">
         <v>23</v>
       </c>
-      <c r="I41" t="s">
-        <v>21</v>
-      </c>
       <c r="J41" t="s">
         <v>21</v>
       </c>
@@ -3260,56 +3389,59 @@
       <c r="O41" t="s">
         <v>21</v>
       </c>
-      <c r="P41">
-        <v>1</v>
+      <c r="P41" t="s">
+        <v>21</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="S41">
         <v>600</v>
       </c>
       <c r="T41">
+        <v>600</v>
+      </c>
+      <c r="U41">
         <v>60</v>
       </c>
-      <c r="U41">
+      <c r="V41">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" t="s">
         <v>93</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
         <v>3079</v>
       </c>
-      <c r="E42" s="2">
+      <c r="F42" s="2">
         <v>27273</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>709</v>
       </c>
-      <c r="G42" s="3">
+      <c r="H42" s="3">
         <v>447</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>51</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>135</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>311</v>
       </c>
-      <c r="K42" t="s">
-        <v>21</v>
-      </c>
       <c r="L42" t="s">
         <v>21</v>
       </c>
@@ -3322,50 +3454,53 @@
       <c r="O42" t="s">
         <v>21</v>
       </c>
-      <c r="P42">
-        <v>1</v>
+      <c r="P42" t="s">
+        <v>21</v>
       </c>
       <c r="Q42">
         <v>1</v>
       </c>
-      <c r="R42" s="1">
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="S42" s="1">
         <v>1020</v>
       </c>
-      <c r="S42" t="s">
-        <v>21</v>
-      </c>
-      <c r="T42">
+      <c r="T42" t="s">
+        <v>21</v>
+      </c>
+      <c r="U42">
         <v>35</v>
       </c>
-      <c r="U42">
+      <c r="V42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
         <v>95</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
         <v>1559</v>
       </c>
-      <c r="E43" s="2">
+      <c r="F43" s="2">
         <v>30225</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>96</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="H43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" t="s">
         <v>23</v>
       </c>
-      <c r="I43" t="s">
-        <v>21</v>
-      </c>
       <c r="J43" t="s">
         <v>21</v>
       </c>
@@ -3384,50 +3519,53 @@
       <c r="O43" t="s">
         <v>21</v>
       </c>
-      <c r="P43">
-        <v>1</v>
+      <c r="P43" t="s">
+        <v>21</v>
       </c>
       <c r="Q43">
         <v>1</v>
       </c>
-      <c r="R43" t="s">
-        <v>21</v>
+      <c r="R43">
+        <v>1</v>
       </c>
       <c r="S43" t="s">
         <v>21</v>
       </c>
-      <c r="T43">
+      <c r="T43" t="s">
+        <v>21</v>
+      </c>
+      <c r="U43">
         <v>39</v>
       </c>
-      <c r="U43">
+      <c r="V43">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
         <v>97</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="D44">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="E44">
         <v>198</v>
       </c>
-      <c r="E44" s="2">
+      <c r="F44" s="2">
         <v>31837</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>65</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="H44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" t="s">
         <v>23</v>
       </c>
-      <c r="I44" t="s">
-        <v>21</v>
-      </c>
       <c r="J44" t="s">
         <v>21</v>
       </c>
@@ -3446,56 +3584,59 @@
       <c r="O44" t="s">
         <v>21</v>
       </c>
-      <c r="P44">
-        <v>1</v>
+      <c r="P44" t="s">
+        <v>21</v>
       </c>
       <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="R44" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
       </c>
       <c r="S44" t="s">
         <v>21</v>
       </c>
-      <c r="T44">
+      <c r="T44" t="s">
+        <v>21</v>
+      </c>
+      <c r="U44">
         <v>12</v>
       </c>
-      <c r="U44" t="s">
+      <c r="V44" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
         <v>98</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
         <v>2029</v>
       </c>
-      <c r="E45" s="2">
+      <c r="F45" s="2">
         <v>25082</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>628</v>
       </c>
-      <c r="G45" s="3">
+      <c r="H45" s="3">
         <v>334</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>31</v>
       </c>
-      <c r="I45">
-        <v>103</v>
-      </c>
       <c r="J45">
+        <v>103</v>
+      </c>
+      <c r="K45">
         <v>122</v>
       </c>
-      <c r="K45" t="s">
-        <v>21</v>
-      </c>
       <c r="L45" t="s">
         <v>21</v>
       </c>
@@ -3508,270 +3649,339 @@
       <c r="O45" t="s">
         <v>21</v>
       </c>
-      <c r="P45">
-        <v>1</v>
+      <c r="P45" t="s">
+        <v>21</v>
       </c>
       <c r="Q45">
         <v>1</v>
       </c>
       <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
         <v>820</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>900</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>35</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" t="s">
         <v>26</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
         <v>28</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" t="s">
         <v>32</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
         <v>34</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
         <v>35</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
         <v>37</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
         <v>39</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
         <v>40</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" t="s">
         <v>41</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
         <v>42</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" t="s">
         <v>54</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
         <v>62</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" t="s">
         <v>64</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" t="s">
         <v>69</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" t="s">
         <v>69</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" t="s">
         <v>76</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" t="s">
         <v>79</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
         <v>82</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" t="s">
         <v>84</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" t="s">
         <v>94</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" t="s">
         <v>97</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U71">
-    <sortCondition ref="B1"/>
+  <sortState ref="B2:V71">
+    <sortCondition ref="C1"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>